<commit_message>
Added Eric examples to test in SoapUI to plan
</commit_message>
<xml_diff>
--- a/MadJavaTeamBeta Group Project Plan.xlsx
+++ b/MadJavaTeamBeta Group Project Plan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Objective</t>
   </si>
@@ -69,6 +69,12 @@
   </si>
   <si>
     <t>?</t>
+  </si>
+  <si>
+    <t>A sample using RegEx and  Java wrapped as web services</t>
+  </si>
+  <si>
+    <t>Eric put these into a repository to try with SoapUI. Mitch and Dave joined. Will test these and consider an additional use of the apache commons pre-built validator as a Web Service.</t>
   </si>
 </sst>
 </file>
@@ -120,13 +126,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -411,7 +420,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,12 +491,15 @@
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" s="3"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B10" s="3">
         <v>42303</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add testing repo version and notes - Dave
</commit_message>
<xml_diff>
--- a/MadJavaTeamBeta Group Project Plan.xlsx
+++ b/MadJavaTeamBeta Group Project Plan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Objective</t>
   </si>
@@ -75,13 +75,37 @@
   </si>
   <si>
     <t>Eric put these into a repository to try with SoapUI. Mitch and Dave joined. Will test these and consider an additional use of the apache commons pre-built validator as a Web Service.</t>
+  </si>
+  <si>
+    <t>Test the WebServices Eric created</t>
+  </si>
+  <si>
+    <t>Dave - worked great, but thought we should add methods to return a String.  I also created the repo to test the String results and used the built-in jersey server. Put these in EmailValidationRestTest.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dbsullivan@madisoncollege </t>
+  </si>
+  <si>
+    <t>Test result Differences noted:</t>
+  </si>
+  <si>
+    <t>isEmailValid (InternetAddress)</t>
+  </si>
+  <si>
+    <t>isEmailValid2 (RegEx)</t>
+  </si>
+  <si>
+    <t>When I setup tests, I noticed user might want to combine tests to avoid conflicting results. Regex might be more accurate when extension is omitted.</t>
+  </si>
+  <si>
+    <t>I plan to put this into my TennisApp as an edit on Player entry</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,6 +129,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -123,10 +155,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -137,8 +170,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -417,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -428,17 +468,17 @@
     <col min="1" max="1" width="55" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="59.140625" customWidth="1"/>
-    <col min="4" max="4" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" customWidth="1"/>
     <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -449,7 +489,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
@@ -457,10 +497,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -471,27 +511,27 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="3"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="3"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="3"/>
     </row>
-    <row r="10" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -502,40 +542,98 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="3"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="3">
+        <v>42303</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B12" s="3">
+        <v>42303</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="3">
+        <v>42303</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="3"/>
+      <c r="C14" s="5"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="3">
+        <v>42310</v>
+      </c>
+      <c r="C15" s="5"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="3"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B17" s="3">
         <v>42310</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B13" s="3"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B15" s="3"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="3"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="3"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="3"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+      <c r="B22" s="3"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B24" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C24" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C13" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>